<commit_message>
RSD: Use IE and National instead of Allregions and include R-HC*
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_RSD_UnitBoilers.xlsx
@@ -5,18 +5,38 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E4SMA-7\Documents\E4SMA Collaborazioni\UCC\20210215_SubRES RSD review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F684FFC3-C0AC-4739-8DF4-A6C77BF97A5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C98577-F1D0-4339-9DF5-C83EEACA2BE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
-    <sheet name="UC unit boilers" sheetId="1" r:id="rId1"/>
+    <sheet name="Regions" sheetId="2" r:id="rId1"/>
+    <sheet name="UC unit boilers" sheetId="1" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'UC unit boilers'!$A$7:$H$13</definedName>
+    <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'UC unit boilers'!$A$7:$H$13</definedName>
+    <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
+    <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,8 +56,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -108,18 +150,220 @@
     <t>Linking Dwellings and Boilers</t>
   </si>
   <si>
-    <t>~UC_Sets: R_E: AllRegions</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://en.wikipedia.org/wiki/ISO_3166-2:IE</t>
+    </r>
+  </si>
+  <si>
+    <t>Wicklow</t>
+  </si>
+  <si>
+    <t>IE-WW</t>
+  </si>
+  <si>
+    <t>Wexford</t>
+  </si>
+  <si>
+    <t>IE-WX</t>
+  </si>
+  <si>
+    <t>Westmeath</t>
+  </si>
+  <si>
+    <t>IE-WH</t>
+  </si>
+  <si>
+    <t>Waterford</t>
+  </si>
+  <si>
+    <t>IE-WD</t>
+  </si>
+  <si>
+    <t>Tipperary</t>
+  </si>
+  <si>
+    <t>IE-TA</t>
+  </si>
+  <si>
+    <t>Sligo</t>
+  </si>
+  <si>
+    <t>IE-SO</t>
+  </si>
+  <si>
+    <t>Roscommon</t>
+  </si>
+  <si>
+    <t>IE-RN</t>
+  </si>
+  <si>
+    <t>Offaly</t>
+  </si>
+  <si>
+    <t>IE-OY</t>
+  </si>
+  <si>
+    <t>Monaghan</t>
+  </si>
+  <si>
+    <t>IE-MN</t>
+  </si>
+  <si>
+    <t>Meath</t>
+  </si>
+  <si>
+    <t>IE-MH</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>IE-MO</t>
+  </si>
+  <si>
+    <t>Louth</t>
+  </si>
+  <si>
+    <t>IE-LH</t>
+  </si>
+  <si>
+    <t>Longford</t>
+  </si>
+  <si>
+    <t>IE-LD</t>
+  </si>
+  <si>
+    <t>Limerick</t>
+  </si>
+  <si>
+    <t>IE-LK</t>
+  </si>
+  <si>
+    <t>Leitrim</t>
+  </si>
+  <si>
+    <t>IE-LM</t>
+  </si>
+  <si>
+    <t>Laois</t>
+  </si>
+  <si>
+    <t>IE-LS</t>
+  </si>
+  <si>
+    <t>Kilkenny</t>
+  </si>
+  <si>
+    <t>IE-KK</t>
+  </si>
+  <si>
+    <t>Kildare</t>
+  </si>
+  <si>
+    <t>IE-KE</t>
+  </si>
+  <si>
+    <t>Kerry</t>
+  </si>
+  <si>
+    <t>IE-KY</t>
+  </si>
+  <si>
+    <t>Galway</t>
+  </si>
+  <si>
+    <t>IE-G</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>IE-D</t>
+  </si>
+  <si>
+    <t>Donegal</t>
+  </si>
+  <si>
+    <t>IE-DL</t>
+  </si>
+  <si>
+    <t>Cork</t>
+  </si>
+  <si>
+    <t>IE-CO</t>
+  </si>
+  <si>
+    <t>Clare</t>
+  </si>
+  <si>
+    <t>IE-CE</t>
+  </si>
+  <si>
+    <t>Cavan</t>
+  </si>
+  <si>
+    <t>IE-CN</t>
+  </si>
+  <si>
+    <t>Carlow</t>
+  </si>
+  <si>
+    <t>IE-CW</t>
+  </si>
+  <si>
+    <t>County name</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Multi-region</t>
+  </si>
+  <si>
+    <t>Single-region</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Development</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -168,8 +412,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,8 +434,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -222,39 +486,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10 2 2 2 2 2" xfId="1" xr:uid="{48456FE6-B823-4B8E-BA2E-F82418748F3D}"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{7E5436E8-2590-4632-AACB-4BBC63308D76}"/>
     <cellStyle name="Normal 4 2 3 4" xfId="2" xr:uid="{D3DDFA03-D001-49FA-BDB2-8EF215704201}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -268,6 +585,81 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="39" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="828675" cy="190500"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Drop Down 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AB3B88C-1B4C-4E5C-B16C-7FF680B9C3C7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="UC_ModalShares"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -566,6 +958,772 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B609416A-93FB-47DC-AE22-6A4361BED7B1}">
+  <dimension ref="A3:AD37"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="8" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="6" style="8" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C3" s="13" t="str" cm="1">
+        <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
+        <v>IE</v>
+      </c>
+      <c r="D3" s="13" t="str" cm="1">
+        <f t="array" ref="D3">INDEX(D5:D7,$A$4)</f>
+        <v>National</v>
+      </c>
+      <c r="E3" s="13" t="str" cm="1">
+        <f t="array" ref="E3">INDEX(E5:E7,$A$4)</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F3" s="13" t="str" cm="1">
+        <f t="array" ref="F3">INDEX(F5:F7,$A$4)</f>
+        <v>IE-D</v>
+      </c>
+      <c r="G3" s="13" t="str" cm="1">
+        <f t="array" ref="G3">INDEX(G5:G7,$A$4)</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="H3" s="13" t="str" cm="1">
+        <f t="array" ref="H3">INDEX(H5:H7,$A$4)</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="I3" s="13" t="str" cm="1">
+        <f t="array" ref="I3">INDEX(I5:I7,$A$4)</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="J3" s="13" t="str" cm="1">
+        <f t="array" ref="J3">INDEX(J5:J7,$A$4)</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="K3" s="13" t="str" cm="1">
+        <f t="array" ref="K3">INDEX(K5:K7,$A$4)</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="L3" s="13" t="str" cm="1">
+        <f t="array" ref="L3">INDEX(L5:L7,$A$4)</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="M3" s="13" t="str" cm="1">
+        <f t="array" ref="M3">INDEX(M5:M7,$A$4)</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="N3" s="13" t="str" cm="1">
+        <f t="array" ref="N3">INDEX(N5:N7,$A$4)</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="O3" s="13" t="str" cm="1">
+        <f t="array" ref="O3">INDEX(O5:O7,$A$4)</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="P3" s="13" t="str" cm="1">
+        <f t="array" ref="P3">INDEX(P5:P7,$A$4)</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q3" s="13" t="str" cm="1">
+        <f t="array" ref="Q3">INDEX(Q5:Q7,$A$4)</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="R3" s="13" t="str" cm="1">
+        <f t="array" ref="R3">INDEX(R5:R7,$A$4)</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="S3" s="13" t="str" cm="1">
+        <f t="array" ref="S3">INDEX(S5:S7,$A$4)</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="T3" s="13" t="str" cm="1">
+        <f t="array" ref="T3">INDEX(T5:T7,$A$4)</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="U3" s="13" t="str" cm="1">
+        <f t="array" ref="U3">INDEX(U5:U7,$A$4)</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="V3" s="13" t="str" cm="1">
+        <f t="array" ref="V3">INDEX(V5:V7,$A$4)</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="W3" s="13" t="str" cm="1">
+        <f t="array" ref="W3">INDEX(W5:W7,$A$4)</f>
+        <v>IE-G</v>
+      </c>
+      <c r="X3" s="13" t="str" cm="1">
+        <f t="array" ref="X3">INDEX(X5:X7,$A$4)</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y3" s="13" t="str" cm="1">
+        <f t="array" ref="Y3">INDEX(Y5:Y7,$A$4)</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z3" s="13" t="str" cm="1">
+        <f t="array" ref="Z3">INDEX(Z5:Z7,$A$4)</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA3" s="13" t="str" cm="1">
+        <f t="array" ref="AA3">INDEX(AA5:AA7,$A$4)</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB3" s="13" t="str" cm="1">
+        <f t="array" ref="AB3">INDEX(AB5:AB7,$A$4)</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC3" s="13" t="str" cm="1">
+        <f t="array" ref="AC3">INDEX(AC5:AC7,$A$4)</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD3" s="13" t="str" cm="1">
+        <f t="array" ref="AD3">INDEX(AD5:AD7,$A$4)</f>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f>Regions!A11</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F5" s="13" t="str">
+        <f>Regions!A16</f>
+        <v>IE-D</v>
+      </c>
+      <c r="G5" s="13" t="str">
+        <f>Regions!A19</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="H5" s="13" t="str">
+        <f>Regions!A20</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="I5" s="13" t="str">
+        <f>Regions!A21</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="J5" s="13" t="str">
+        <f>Regions!A24</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="K5" s="13" t="str">
+        <f>Regions!A25</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="L5" s="13" t="str">
+        <f>Regions!A27</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="M5" s="13" t="str">
+        <f>Regions!A29</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="N5" s="13" t="str">
+        <f>Regions!A34</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="O5" s="13" t="str">
+        <f>Regions!A35</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="P5" s="13" t="str">
+        <f>Regions!A36</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q5" s="13" t="str">
+        <f>Regions!A13</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="R5" s="13" t="str">
+        <f>Regions!A14</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="S5" s="13" t="str">
+        <f>Regions!A18</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="T5" s="13" t="str">
+        <f>Regions!A23</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="U5" s="13" t="str">
+        <f>Regions!A32</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="V5" s="13" t="str">
+        <f>Regions!A33</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="W5" s="13" t="str">
+        <f>Regions!A17</f>
+        <v>IE-G</v>
+      </c>
+      <c r="X5" s="13" t="str">
+        <f>Regions!A22</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y5" s="13" t="str">
+        <f>Regions!A26</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z5" s="13" t="str">
+        <f>Regions!A30</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA5" s="13" t="str">
+        <f>Regions!A31</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB5" s="13" t="str">
+        <f>Regions!A12</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC5" s="13" t="str">
+        <f>Regions!A15</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD5" s="13" t="str">
+        <f>Regions!A28</f>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="13" t="str">
+        <f>C5</f>
+        <v>IE</v>
+      </c>
+      <c r="D6" s="13" t="str">
+        <f>"*"&amp;D5</f>
+        <v>*National</v>
+      </c>
+      <c r="E6" s="13" t="str">
+        <f>"*"&amp;E5</f>
+        <v>*IE-CW</v>
+      </c>
+      <c r="F6" s="13" t="str">
+        <f>"*"&amp;F5</f>
+        <v>*IE-D</v>
+      </c>
+      <c r="G6" s="13" t="str">
+        <f>"*"&amp;G5</f>
+        <v>*IE-KE</v>
+      </c>
+      <c r="H6" s="13" t="str">
+        <f>"*"&amp;H5</f>
+        <v>*IE-KK</v>
+      </c>
+      <c r="I6" s="13" t="str">
+        <f>"*"&amp;I5</f>
+        <v>*IE-LS</v>
+      </c>
+      <c r="J6" s="13" t="str">
+        <f>"*"&amp;J5</f>
+        <v>*IE-LD</v>
+      </c>
+      <c r="K6" s="13" t="str">
+        <f>"*"&amp;K5</f>
+        <v>*IE-LH</v>
+      </c>
+      <c r="L6" s="13" t="str">
+        <f>"*"&amp;L5</f>
+        <v>*IE-MH</v>
+      </c>
+      <c r="M6" s="13" t="str">
+        <f>"*"&amp;M5</f>
+        <v>*IE-OY</v>
+      </c>
+      <c r="N6" s="13" t="str">
+        <f>"*"&amp;N5</f>
+        <v>*IE-WH</v>
+      </c>
+      <c r="O6" s="13" t="str">
+        <f>"*"&amp;O5</f>
+        <v>*IE-WX</v>
+      </c>
+      <c r="P6" s="13" t="str">
+        <f>"*"&amp;P5</f>
+        <v>*IE-WW</v>
+      </c>
+      <c r="Q6" s="13" t="str">
+        <f>"*"&amp;Q5</f>
+        <v>*IE-CE</v>
+      </c>
+      <c r="R6" s="13" t="str">
+        <f>"*"&amp;R5</f>
+        <v>*IE-CO</v>
+      </c>
+      <c r="S6" s="13" t="str">
+        <f>"*"&amp;S5</f>
+        <v>*IE-KY</v>
+      </c>
+      <c r="T6" s="13" t="str">
+        <f>"*"&amp;T5</f>
+        <v>*IE-LK</v>
+      </c>
+      <c r="U6" s="13" t="str">
+        <f>"*"&amp;U5</f>
+        <v>*IE-TA</v>
+      </c>
+      <c r="V6" s="13" t="str">
+        <f>"*"&amp;V5</f>
+        <v>*IE-WD</v>
+      </c>
+      <c r="W6" s="13" t="str">
+        <f>"*"&amp;W5</f>
+        <v>*IE-G</v>
+      </c>
+      <c r="X6" s="13" t="str">
+        <f>"*"&amp;X5</f>
+        <v>*IE-LM</v>
+      </c>
+      <c r="Y6" s="13" t="str">
+        <f>"*"&amp;Y5</f>
+        <v>*IE-MO</v>
+      </c>
+      <c r="Z6" s="13" t="str">
+        <f>"*"&amp;Z5</f>
+        <v>*IE-RN</v>
+      </c>
+      <c r="AA6" s="13" t="str">
+        <f>"*"&amp;AA5</f>
+        <v>*IE-SO</v>
+      </c>
+      <c r="AB6" s="13" t="str">
+        <f>"*"&amp;AB5</f>
+        <v>*IE-CN</v>
+      </c>
+      <c r="AC6" s="13" t="str">
+        <f>"*"&amp;AC5</f>
+        <v>*IE-DL</v>
+      </c>
+      <c r="AD6" s="13" t="str">
+        <f>"*"&amp;AD5</f>
+        <v>*IE-MN</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="13" t="str">
+        <f>"*"&amp;C5</f>
+        <v>*IE</v>
+      </c>
+      <c r="D7" s="13" t="str">
+        <f>D5</f>
+        <v>National</v>
+      </c>
+      <c r="E7" s="13" t="str">
+        <f>E5</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F7" s="13" t="str">
+        <f>F5</f>
+        <v>IE-D</v>
+      </c>
+      <c r="G7" s="13" t="str">
+        <f>G5</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="H7" s="13" t="str">
+        <f>H5</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="I7" s="13" t="str">
+        <f>I5</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="J7" s="13" t="str">
+        <f>J5</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="K7" s="13" t="str">
+        <f>K5</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="L7" s="13" t="str">
+        <f>L5</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="M7" s="13" t="str">
+        <f>M5</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="N7" s="13" t="str">
+        <f>N5</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="O7" s="13" t="str">
+        <f>O5</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="P7" s="13" t="str">
+        <f>P5</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q7" s="13" t="str">
+        <f>Q5</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="R7" s="13" t="str">
+        <f>R5</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="S7" s="13" t="str">
+        <f>S5</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="T7" s="13" t="str">
+        <f>T5</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="U7" s="13" t="str">
+        <f>U5</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="V7" s="13" t="str">
+        <f>V5</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="W7" s="13" t="str">
+        <f>W5</f>
+        <v>IE-G</v>
+      </c>
+      <c r="X7" s="13" t="str">
+        <f>X5</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y7" s="13" t="str">
+        <f>Y5</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z7" s="13" t="str">
+        <f>Z5</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA7" s="13" t="str">
+        <f>AA5</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB7" s="13" t="str">
+        <f>AB5</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC7" s="13" t="str">
+        <f>AC5</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD7" s="13" t="str">
+        <f>AD5</f>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId4" name="Drop Down 1">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B514644-E1CE-4A77-88F5-320229FB7B63}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
@@ -573,14 +1731,14 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="8.42578125" style="2" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -598,8 +1756,9 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
+      <c r="A4" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
+        <v>~UC_Sets: R_E: IE,National</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -655,8 +1814,8 @@
         <v>Minimum number of boilers for RSD Apt</v>
       </c>
       <c r="C8" s="2" t="str">
-        <f>"R-SH_"&amp;J8&amp;"*, "&amp;"R-SW_"&amp;J8&amp;"*, "&amp;"R-SC_"&amp;J8&amp;"*"</f>
-        <v>R-SH_Apt*, R-SW_Apt*, R-SC_Apt*</v>
+        <f>"R-SH_"&amp;J8&amp;"*, "&amp;"R-SW_"&amp;J8&amp;"*, "&amp;"R-SC_"&amp;J8&amp;"*,"&amp;"R-HC_"&amp;J8&amp;"*"</f>
+        <v>R-SH_Apt*, R-SW_Apt*, R-SC_Apt*,R-HC_Apt*</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>"RSDSH_"&amp;J8</f>
@@ -699,8 +1858,8 @@
         <v>Minimum number of boilers for RSD Att</v>
       </c>
       <c r="C10" s="2" t="str">
-        <f>"R-SH_"&amp;J10&amp;"*, "&amp;"R-SW_"&amp;J10&amp;"*, "&amp;"R-SC_"&amp;J10&amp;"*"</f>
-        <v>R-SH_Att*, R-SW_Att*, R-SC_Att*</v>
+        <f>"R-SH_"&amp;J10&amp;"*, "&amp;"R-SW_"&amp;J10&amp;"*, "&amp;"R-SC_"&amp;J10&amp;"*,"&amp;"R-HC_"&amp;J10&amp;"*"</f>
+        <v>R-SH_Att*, R-SW_Att*, R-SC_Att*,R-HC_Att*</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>"RSDSH_"&amp;J10</f>
@@ -743,8 +1902,8 @@
         <v>Minimum number of boilers for RSD Det</v>
       </c>
       <c r="C12" s="2" t="str">
-        <f>"R-SH_"&amp;J12&amp;"*, "&amp;"R-SW_"&amp;J12&amp;"*, "&amp;"R-SC_"&amp;J12&amp;"*"</f>
-        <v>R-SH_Det*, R-SW_Det*, R-SC_Det*</v>
+        <f>"R-SH_"&amp;J12&amp;"*, "&amp;"R-SW_"&amp;J12&amp;"*, "&amp;"R-SC_"&amp;J12&amp;"*,"&amp;"R-HC_"&amp;J12&amp;"*"</f>
+        <v>R-SH_Det*, R-SW_Det*, R-SC_Det*,R-HC_Det*</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>"RSDSH_"&amp;J12</f>

</xml_diff>

<commit_message>
Make number of boilers equal number of dwellings
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_RSD_UnitBoilers.xlsx
@@ -8,17 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C98577-F1D0-4339-9DF5-C83EEACA2BE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A86A4B-3500-44CF-A53B-D29B92C94875}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
     <sheet name="UC unit boilers" sheetId="1" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'UC unit boilers'!$A$7:$H$13</definedName>
@@ -105,9 +102,6 @@
     <t>UC_Desc</t>
   </si>
   <si>
-    <t>LO</t>
-  </si>
-  <si>
     <t>Att</t>
   </si>
   <si>
@@ -346,6 +340,9 @@
   </si>
   <si>
     <t>Development</t>
+  </si>
+  <si>
+    <t>FX</t>
   </si>
 </sst>
 </file>
@@ -595,14 +592,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="828675" cy="190500"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>19050</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1025" name="Drop Down 1" hidden="1">
@@ -611,7 +613,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AB3B88C-1B4C-4E5C-B16C-7FF680B9C3C7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -642,24 +644,11 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="UC_ModalShares"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1119,13 +1108,13 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="13" t="str">
         <f>Regions!A11</f>
@@ -1234,457 +1223,457 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="13" t="str">
         <f>C5</f>
         <v>IE</v>
       </c>
       <c r="D6" s="13" t="str">
-        <f>"*"&amp;D5</f>
+        <f t="shared" ref="D6:AD6" si="0">"*"&amp;D5</f>
         <v>*National</v>
       </c>
       <c r="E6" s="13" t="str">
-        <f>"*"&amp;E5</f>
+        <f t="shared" si="0"/>
         <v>*IE-CW</v>
       </c>
       <c r="F6" s="13" t="str">
-        <f>"*"&amp;F5</f>
+        <f t="shared" si="0"/>
         <v>*IE-D</v>
       </c>
       <c r="G6" s="13" t="str">
-        <f>"*"&amp;G5</f>
+        <f t="shared" si="0"/>
         <v>*IE-KE</v>
       </c>
       <c r="H6" s="13" t="str">
-        <f>"*"&amp;H5</f>
+        <f t="shared" si="0"/>
         <v>*IE-KK</v>
       </c>
       <c r="I6" s="13" t="str">
-        <f>"*"&amp;I5</f>
+        <f t="shared" si="0"/>
         <v>*IE-LS</v>
       </c>
       <c r="J6" s="13" t="str">
-        <f>"*"&amp;J5</f>
+        <f t="shared" si="0"/>
         <v>*IE-LD</v>
       </c>
       <c r="K6" s="13" t="str">
-        <f>"*"&amp;K5</f>
+        <f t="shared" si="0"/>
         <v>*IE-LH</v>
       </c>
       <c r="L6" s="13" t="str">
-        <f>"*"&amp;L5</f>
+        <f t="shared" si="0"/>
         <v>*IE-MH</v>
       </c>
       <c r="M6" s="13" t="str">
-        <f>"*"&amp;M5</f>
+        <f t="shared" si="0"/>
         <v>*IE-OY</v>
       </c>
       <c r="N6" s="13" t="str">
-        <f>"*"&amp;N5</f>
+        <f t="shared" si="0"/>
         <v>*IE-WH</v>
       </c>
       <c r="O6" s="13" t="str">
-        <f>"*"&amp;O5</f>
+        <f t="shared" si="0"/>
         <v>*IE-WX</v>
       </c>
       <c r="P6" s="13" t="str">
-        <f>"*"&amp;P5</f>
+        <f t="shared" si="0"/>
         <v>*IE-WW</v>
       </c>
       <c r="Q6" s="13" t="str">
-        <f>"*"&amp;Q5</f>
+        <f t="shared" si="0"/>
         <v>*IE-CE</v>
       </c>
       <c r="R6" s="13" t="str">
-        <f>"*"&amp;R5</f>
+        <f t="shared" si="0"/>
         <v>*IE-CO</v>
       </c>
       <c r="S6" s="13" t="str">
-        <f>"*"&amp;S5</f>
+        <f t="shared" si="0"/>
         <v>*IE-KY</v>
       </c>
       <c r="T6" s="13" t="str">
-        <f>"*"&amp;T5</f>
+        <f t="shared" si="0"/>
         <v>*IE-LK</v>
       </c>
       <c r="U6" s="13" t="str">
-        <f>"*"&amp;U5</f>
+        <f t="shared" si="0"/>
         <v>*IE-TA</v>
       </c>
       <c r="V6" s="13" t="str">
-        <f>"*"&amp;V5</f>
+        <f t="shared" si="0"/>
         <v>*IE-WD</v>
       </c>
       <c r="W6" s="13" t="str">
-        <f>"*"&amp;W5</f>
+        <f t="shared" si="0"/>
         <v>*IE-G</v>
       </c>
       <c r="X6" s="13" t="str">
-        <f>"*"&amp;X5</f>
+        <f t="shared" si="0"/>
         <v>*IE-LM</v>
       </c>
       <c r="Y6" s="13" t="str">
-        <f>"*"&amp;Y5</f>
+        <f t="shared" si="0"/>
         <v>*IE-MO</v>
       </c>
       <c r="Z6" s="13" t="str">
-        <f>"*"&amp;Z5</f>
+        <f t="shared" si="0"/>
         <v>*IE-RN</v>
       </c>
       <c r="AA6" s="13" t="str">
-        <f>"*"&amp;AA5</f>
+        <f t="shared" si="0"/>
         <v>*IE-SO</v>
       </c>
       <c r="AB6" s="13" t="str">
-        <f>"*"&amp;AB5</f>
+        <f t="shared" si="0"/>
         <v>*IE-CN</v>
       </c>
       <c r="AC6" s="13" t="str">
-        <f>"*"&amp;AC5</f>
+        <f t="shared" si="0"/>
         <v>*IE-DL</v>
       </c>
       <c r="AD6" s="13" t="str">
-        <f>"*"&amp;AD5</f>
+        <f t="shared" si="0"/>
         <v>*IE-MN</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="13" t="str">
         <f>"*"&amp;C5</f>
         <v>*IE</v>
       </c>
       <c r="D7" s="13" t="str">
-        <f>D5</f>
+        <f t="shared" ref="D7:AD7" si="1">D5</f>
         <v>National</v>
       </c>
       <c r="E7" s="13" t="str">
-        <f>E5</f>
+        <f t="shared" si="1"/>
         <v>IE-CW</v>
       </c>
       <c r="F7" s="13" t="str">
-        <f>F5</f>
+        <f t="shared" si="1"/>
         <v>IE-D</v>
       </c>
       <c r="G7" s="13" t="str">
-        <f>G5</f>
+        <f t="shared" si="1"/>
         <v>IE-KE</v>
       </c>
       <c r="H7" s="13" t="str">
-        <f>H5</f>
+        <f t="shared" si="1"/>
         <v>IE-KK</v>
       </c>
       <c r="I7" s="13" t="str">
-        <f>I5</f>
+        <f t="shared" si="1"/>
         <v>IE-LS</v>
       </c>
       <c r="J7" s="13" t="str">
-        <f>J5</f>
+        <f t="shared" si="1"/>
         <v>IE-LD</v>
       </c>
       <c r="K7" s="13" t="str">
-        <f>K5</f>
+        <f t="shared" si="1"/>
         <v>IE-LH</v>
       </c>
       <c r="L7" s="13" t="str">
-        <f>L5</f>
+        <f t="shared" si="1"/>
         <v>IE-MH</v>
       </c>
       <c r="M7" s="13" t="str">
-        <f>M5</f>
+        <f t="shared" si="1"/>
         <v>IE-OY</v>
       </c>
       <c r="N7" s="13" t="str">
-        <f>N5</f>
+        <f t="shared" si="1"/>
         <v>IE-WH</v>
       </c>
       <c r="O7" s="13" t="str">
-        <f>O5</f>
+        <f t="shared" si="1"/>
         <v>IE-WX</v>
       </c>
       <c r="P7" s="13" t="str">
-        <f>P5</f>
+        <f t="shared" si="1"/>
         <v>IE-WW</v>
       </c>
       <c r="Q7" s="13" t="str">
-        <f>Q5</f>
+        <f t="shared" si="1"/>
         <v>IE-CE</v>
       </c>
       <c r="R7" s="13" t="str">
-        <f>R5</f>
+        <f t="shared" si="1"/>
         <v>IE-CO</v>
       </c>
       <c r="S7" s="13" t="str">
-        <f>S5</f>
+        <f t="shared" si="1"/>
         <v>IE-KY</v>
       </c>
       <c r="T7" s="13" t="str">
-        <f>T5</f>
+        <f t="shared" si="1"/>
         <v>IE-LK</v>
       </c>
       <c r="U7" s="13" t="str">
-        <f>U5</f>
+        <f t="shared" si="1"/>
         <v>IE-TA</v>
       </c>
       <c r="V7" s="13" t="str">
-        <f>V5</f>
+        <f t="shared" si="1"/>
         <v>IE-WD</v>
       </c>
       <c r="W7" s="13" t="str">
-        <f>W5</f>
+        <f t="shared" si="1"/>
         <v>IE-G</v>
       </c>
       <c r="X7" s="13" t="str">
-        <f>X5</f>
+        <f t="shared" si="1"/>
         <v>IE-LM</v>
       </c>
       <c r="Y7" s="13" t="str">
-        <f>Y5</f>
+        <f t="shared" si="1"/>
         <v>IE-MO</v>
       </c>
       <c r="Z7" s="13" t="str">
-        <f>Z5</f>
+        <f t="shared" si="1"/>
         <v>IE-RN</v>
       </c>
       <c r="AA7" s="13" t="str">
-        <f>AA5</f>
+        <f t="shared" si="1"/>
         <v>IE-SO</v>
       </c>
       <c r="AB7" s="13" t="str">
-        <f>AB5</f>
+        <f t="shared" si="1"/>
         <v>IE-CN</v>
       </c>
       <c r="AC7" s="13" t="str">
-        <f>AC5</f>
+        <f t="shared" si="1"/>
         <v>IE-DL</v>
       </c>
       <c r="AD7" s="13" t="str">
-        <f>AD5</f>
+        <f t="shared" si="1"/>
         <v>IE-MN</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1731,13 +1720,13 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="8.42578125" style="2" customWidth="1"/>
@@ -1747,12 +1736,12 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -1782,10 +1771,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>3</v>
@@ -1801,7 +1790,7 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1810,19 +1799,19 @@
         <v>UC_RSD_UnitBoiler-Apt</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f>"Minimum number of boilers for RSD "&amp;J8</f>
-        <v>Minimum number of boilers for RSD Apt</v>
+        <f>"Number of boilers equals number of dwellings in RSD "&amp;J8</f>
+        <v>Number of boilers equals number of dwellings in RSD Apt</v>
       </c>
       <c r="C8" s="2" t="str">
-        <f>"R-SH_"&amp;J8&amp;"*, "&amp;"R-SW_"&amp;J8&amp;"*, "&amp;"R-SC_"&amp;J8&amp;"*,"&amp;"R-HC_"&amp;J8&amp;"*"</f>
-        <v>R-SH_Apt*, R-SW_Apt*, R-SC_Apt*,R-HC_Apt*</v>
+        <f>"R-SH_"&amp;J8&amp;"*, "&amp;"R-SW_"&amp;J8&amp;"*, "&amp;"R-HC_"&amp;J8&amp;"*"</f>
+        <v>R-SH_Apt*, R-SW_Apt*, R-HC_Apt*</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>"RSDSH_"&amp;J8</f>
         <v>RSDSH_Apt</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
@@ -1835,7 +1824,7 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1854,19 +1843,19 @@
         <v>UC_RSD_UnitBoiler-Att</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f>"Minimum number of boilers for RSD "&amp;J10</f>
-        <v>Minimum number of boilers for RSD Att</v>
+        <f>"Number of boilers equals number of dwellings in RSD "&amp;J10</f>
+        <v>Number of boilers equals number of dwellings in RSD Att</v>
       </c>
       <c r="C10" s="2" t="str">
-        <f>"R-SH_"&amp;J10&amp;"*, "&amp;"R-SW_"&amp;J10&amp;"*, "&amp;"R-SC_"&amp;J10&amp;"*,"&amp;"R-HC_"&amp;J10&amp;"*"</f>
-        <v>R-SH_Att*, R-SW_Att*, R-SC_Att*,R-HC_Att*</v>
+        <f>"R-SH_"&amp;J10&amp;"*, "&amp;"R-SW_"&amp;J10&amp;"*, "&amp;"R-HC_"&amp;J10&amp;"*"</f>
+        <v>R-SH_Att*, R-SW_Att*, R-HC_Att*</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>"RSDSH_"&amp;J10</f>
         <v>RSDSH_Att</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -1879,7 +1868,7 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1898,19 +1887,19 @@
         <v>UC_RSD_UnitBoiler-Det</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f>"Minimum number of boilers for RSD "&amp;J12</f>
-        <v>Minimum number of boilers for RSD Det</v>
+        <f>"Number of boilers equals number of dwellings in RSD "&amp;J12</f>
+        <v>Number of boilers equals number of dwellings in RSD Det</v>
       </c>
       <c r="C12" s="2" t="str">
-        <f>"R-SH_"&amp;J12&amp;"*, "&amp;"R-SW_"&amp;J12&amp;"*, "&amp;"R-SC_"&amp;J12&amp;"*,"&amp;"R-HC_"&amp;J12&amp;"*"</f>
-        <v>R-SH_Det*, R-SW_Det*, R-SC_Det*,R-HC_Det*</v>
+        <f>"R-SH_"&amp;J12&amp;"*, "&amp;"R-SW_"&amp;J12&amp;"*, "&amp;"R-HC_"&amp;J12&amp;"*"</f>
+        <v>R-SH_Det*, R-SW_Det*, R-HC_Det*</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>"RSDSH_"&amp;J12</f>
         <v>RSDSH_Det</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -1923,7 +1912,7 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Extend UnitBoilers constraint to include water heating
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_RSD_UnitBoilers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A86A4B-3500-44CF-A53B-D29B92C94875}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EA0309-39E2-4DEB-AD91-6CBAF843108B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'UC unit boilers'!$A$7:$H$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'UC unit boilers'!$A$7:$I$13</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
     <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>FX</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>*,-*RTFT*</t>
   </si>
 </sst>
 </file>
@@ -1717,53 +1723,54 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="8.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="2" customWidth="1"/>
+    <col min="6" max="9" width="8.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="E6" s="1" t="s">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
@@ -1777,160 +1784,301 @@
         <v>12</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="2"/>
+      <c r="K7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
-        <f>"UC_RSD_UnitBoiler-"&amp;J8</f>
-        <v>UC_RSD_UnitBoiler-Apt</v>
+        <f>"UC_RSD_UnitBoiler_SH-"&amp;K8</f>
+        <v>UC_RSD_UnitBoiler_SH-Apt</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f>"Number of boilers equals number of dwellings in RSD "&amp;J8</f>
-        <v>Number of boilers equals number of dwellings in RSD Apt</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f>"R-SH_"&amp;J8&amp;"*, "&amp;"R-SW_"&amp;J8&amp;"*, "&amp;"R-HC_"&amp;J8&amp;"*"</f>
-        <v>R-SH_Apt*, R-SW_Apt*, R-HC_Apt*</v>
+        <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;K8</f>
+        <v>Number of boilers providing space heat equals number of dwellings in RSD Apt</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f>"RSDSH_"&amp;J8</f>
+        <f>"RSDSH_"&amp;K8</f>
         <v>RSDSH_Apt</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>5</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="str">
-        <f>"R-BLD_"&amp;J8&amp;"*"</f>
+        <f>"R-BLD_"&amp;K8&amp;"*"</f>
         <v>R-BLD_Apt*</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>-1</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
-        <f>"UC_RSD_UnitBoiler-"&amp;J10</f>
-        <v>UC_RSD_UnitBoiler-Att</v>
+        <f>"UC_RSD_UnitBoiler_SH-"&amp;K10</f>
+        <v>UC_RSD_UnitBoiler_SH-Att</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f>"Number of boilers equals number of dwellings in RSD "&amp;J10</f>
-        <v>Number of boilers equals number of dwellings in RSD Att</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f>"R-SH_"&amp;J10&amp;"*, "&amp;"R-SW_"&amp;J10&amp;"*, "&amp;"R-HC_"&amp;J10&amp;"*"</f>
-        <v>R-SH_Att*, R-SW_Att*, R-HC_Att*</v>
+        <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;K10</f>
+        <v>Number of boilers providing space heat equals number of dwellings in RSD Att</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f>"RSDSH_"&amp;J10</f>
+        <f>"RSDSH_"&amp;K10</f>
         <v>RSDSH_Att</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>1</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>0</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>5</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="2"/>
+      <c r="K10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="str">
-        <f>"R-BLD_"&amp;J10&amp;"*"</f>
+        <f>"R-BLD_"&amp;K10&amp;"*"</f>
         <v>R-BLD_Att*</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>-1</v>
       </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
-        <f>"UC_RSD_UnitBoiler-"&amp;J12</f>
-        <v>UC_RSD_UnitBoiler-Det</v>
+        <f>"UC_RSD_UnitBoiler_SH-"&amp;K12</f>
+        <v>UC_RSD_UnitBoiler_SH-Det</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f>"Number of boilers equals number of dwellings in RSD "&amp;J12</f>
-        <v>Number of boilers equals number of dwellings in RSD Det</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f>"R-SH_"&amp;J12&amp;"*, "&amp;"R-SW_"&amp;J12&amp;"*, "&amp;"R-HC_"&amp;J12&amp;"*"</f>
-        <v>R-SH_Det*, R-SW_Det*, R-HC_Det*</v>
+        <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;K12</f>
+        <v>Number of boilers providing space heat equals number of dwellings in RSD Det</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f>"RSDSH_"&amp;J12</f>
+        <f>"RSDSH_"&amp;K12</f>
         <v>RSDSH_Det</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="4">
         <v>0</v>
       </c>
-      <c r="H12" s="4">
+      <c r="I12" s="4">
         <v>5</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="str">
-        <f>"R-BLD_"&amp;J12&amp;"*"</f>
+        <f>"R-BLD_"&amp;K12&amp;"*"</f>
         <v>R-BLD_Det*</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
         <v>-1</v>
       </c>
-      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="str">
+        <f>"UC_RSD_UnitBoiler-HW_"&amp;K14</f>
+        <v>UC_RSD_UnitBoiler-HW_Apt</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f>"Number of boilers providing water heating equals number of dwellings in RSD "&amp;K14</f>
+        <v>Number of boilers providing water heating equals number of dwellings in RSD Apt</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>"RSDWH_"&amp;K14</f>
+        <v>RSDWH_Apt</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>5</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C15" s="2" t="str">
+        <f>"R-BLD_"&amp;K14&amp;"*"</f>
+        <v>R-BLD_Apt*</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="str">
+        <f>"UC_RSD_UnitBoiler-HW_"&amp;K16</f>
+        <v>UC_RSD_UnitBoiler-HW_Att</v>
+      </c>
+      <c r="B16" s="2" t="str">
+        <f>"Number of boiler providing water heatings equals number of dwellings in RSD "&amp;K16</f>
+        <v>Number of boiler providing water heatings equals number of dwellings in RSD Att</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>"RSDWH_"&amp;K16</f>
+        <v>RSDWH_Att</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>5</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="str">
+        <f>"R-BLD_"&amp;K16&amp;"*"</f>
+        <v>R-BLD_Att*</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="str">
+        <f>"UC_RSD_UnitBoiler-HW_"&amp;K18</f>
+        <v>UC_RSD_UnitBoiler-HW_Det</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f>"Number of boilers providing water heating equals number of dwellings in RSD "&amp;K18</f>
+        <v>Number of boilers providing water heating equals number of dwellings in RSD Det</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f>"RSDWH_"&amp;K18</f>
+        <v>RSDWH_Det</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>5</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="str">
+        <f>"R-BLD_"&amp;K18&amp;"*"</f>
+        <v>R-BLD_Det*</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3">
+        <v>-1</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Exclude dummy imports from the UnitBoilers constraint
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_RSD_UnitBoilers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EA0309-39E2-4DEB-AD91-6CBAF843108B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C078F0A-D842-45A1-BB1F-C825E90BE072}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'UC unit boilers'!$A$7:$I$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'UC unit boilers'!$A$7:$J$13</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
     <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t>*,-*RTFT*</t>
+  </si>
+  <si>
+    <t>Pset_set</t>
+  </si>
+  <si>
+    <t>-IRE</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -569,6 +575,9 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1723,10 +1732,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1735,42 +1744,43 @@
     <col min="2" max="2" width="64.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="2" customWidth="1"/>
-    <col min="6" max="9" width="8.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="10.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="2" customWidth="1"/>
+    <col min="7" max="10" width="8.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="F6" s="1" t="s">
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
@@ -1784,301 +1794,324 @@
         <v>12</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="2"/>
+      <c r="L7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
-        <f>"UC_RSD_UnitBoiler_SH-"&amp;K8</f>
+        <f>"UC_RSD_UnitBoiler_SH-"&amp;L8</f>
         <v>UC_RSD_UnitBoiler_SH-Apt</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;K8</f>
+        <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;L8</f>
         <v>Number of boilers providing space heat equals number of dwellings in RSD Apt</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f>"RSDSH_"&amp;K8</f>
+        <f>"RSDSH_"&amp;L8</f>
         <v>RSDSH_Apt</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="2">
         <v>2019</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>1</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>0</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>5</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="str">
-        <f>"R-BLD_"&amp;K8&amp;"*"</f>
+        <f>"R-BLD_"&amp;L8&amp;"*"</f>
         <v>R-BLD_Apt*</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>-1</v>
       </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
-        <f>"UC_RSD_UnitBoiler_SH-"&amp;K10</f>
+        <f>"UC_RSD_UnitBoiler_SH-"&amp;L10</f>
         <v>UC_RSD_UnitBoiler_SH-Att</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;K10</f>
+        <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;L10</f>
         <v>Number of boilers providing space heat equals number of dwellings in RSD Att</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f>"RSDSH_"&amp;K10</f>
+        <f>"RSDSH_"&amp;L10</f>
         <v>RSDSH_Att</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="2">
         <v>2019</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>1</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>0</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>5</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="str">
-        <f>"R-BLD_"&amp;K10&amp;"*"</f>
+        <f>"R-BLD_"&amp;L10&amp;"*"</f>
         <v>R-BLD_Att*</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>-1</v>
       </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
-        <f>"UC_RSD_UnitBoiler_SH-"&amp;K12</f>
+        <f>"UC_RSD_UnitBoiler_SH-"&amp;L12</f>
         <v>UC_RSD_UnitBoiler_SH-Det</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;K12</f>
+        <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;L12</f>
         <v>Number of boilers providing space heat equals number of dwellings in RSD Det</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f>"RSDSH_"&amp;K12</f>
+        <f>"RSDSH_"&amp;L12</f>
         <v>RSDSH_Det</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="2">
         <v>2019</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="4">
         <v>1</v>
       </c>
-      <c r="H12" s="4">
+      <c r="I12" s="4">
         <v>0</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="4">
         <v>5</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="str">
-        <f>"R-BLD_"&amp;K12&amp;"*"</f>
+        <f>"R-BLD_"&amp;L12&amp;"*"</f>
         <v>R-BLD_Det*</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3">
         <v>-1</v>
       </c>
-      <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J13" s="3"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str">
-        <f>"UC_RSD_UnitBoiler-HW_"&amp;K14</f>
+        <f>"UC_RSD_UnitBoiler-HW_"&amp;L14</f>
         <v>UC_RSD_UnitBoiler-HW_Apt</v>
       </c>
       <c r="B14" s="2" t="str">
-        <f>"Number of boilers providing water heating equals number of dwellings in RSD "&amp;K14</f>
+        <f>"Number of boilers providing water heating equals number of dwellings in RSD "&amp;L14</f>
         <v>Number of boilers providing water heating equals number of dwellings in RSD Apt</v>
       </c>
       <c r="D14" s="2" t="str">
-        <f>"RSDWH_"&amp;K14</f>
+        <f>"RSDWH_"&amp;L14</f>
         <v>RSDWH_Apt</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="2">
         <v>2019</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>1</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>0</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>5</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="str">
-        <f>"R-BLD_"&amp;K14&amp;"*"</f>
+        <f>"R-BLD_"&amp;L14&amp;"*"</f>
         <v>R-BLD_Apt*</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="str">
-        <f>"UC_RSD_UnitBoiler-HW_"&amp;K16</f>
+        <f>"UC_RSD_UnitBoiler-HW_"&amp;L16</f>
         <v>UC_RSD_UnitBoiler-HW_Att</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f>"Number of boiler providing water heatings equals number of dwellings in RSD "&amp;K16</f>
+        <f>"Number of boiler providing water heatings equals number of dwellings in RSD "&amp;L16</f>
         <v>Number of boiler providing water heatings equals number of dwellings in RSD Att</v>
       </c>
       <c r="D16" s="2" t="str">
-        <f>"RSDWH_"&amp;K16</f>
+        <f>"RSDWH_"&amp;L16</f>
         <v>RSDWH_Att</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="2">
         <v>2019</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>1</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>0</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>5</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="str">
-        <f>"R-BLD_"&amp;K16&amp;"*"</f>
+        <f>"R-BLD_"&amp;L16&amp;"*"</f>
         <v>R-BLD_Att*</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str">
-        <f>"UC_RSD_UnitBoiler-HW_"&amp;K18</f>
+        <f>"UC_RSD_UnitBoiler-HW_"&amp;L18</f>
         <v>UC_RSD_UnitBoiler-HW_Det</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f>"Number of boilers providing water heating equals number of dwellings in RSD "&amp;K18</f>
+        <f>"Number of boilers providing water heating equals number of dwellings in RSD "&amp;L18</f>
         <v>Number of boilers providing water heating equals number of dwellings in RSD Det</v>
       </c>
       <c r="D18" s="2" t="str">
-        <f>"RSDWH_"&amp;K18</f>
+        <f>"RSDWH_"&amp;L18</f>
         <v>RSDWH_Det</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="2">
         <v>2019</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="4">
+      <c r="H18" s="4">
         <v>1</v>
       </c>
-      <c r="H18" s="4">
+      <c r="I18" s="4">
         <v>0</v>
       </c>
-      <c r="I18" s="4">
+      <c r="J18" s="4">
         <v>5</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="L18" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="str">
-        <f>"R-BLD_"&amp;K18&amp;"*"</f>
+        <f>"R-BLD_"&amp;L18&amp;"*"</f>
         <v>R-BLD_Det*</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="3">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3">
         <v>-1</v>
       </c>
-      <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="L19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add HVO and Fireplaces
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_RSD_UnitBoilers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20DA50E-953E-4202-938E-B2FA89E8ACB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7087BA65-58F7-4A18-A06A-598B7B6CD0FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -347,9 +347,6 @@
     <t>YEAR</t>
   </si>
   <si>
-    <t>*,-*RTFT*</t>
-  </si>
-  <si>
     <t>Pset_set</t>
   </si>
   <si>
@@ -368,7 +365,10 @@
     <t>R*</t>
   </si>
   <si>
-    <t>R-BLD* ALL BUILDINGS</t>
+    <t>*,-*RTFT*,-R*FPL*</t>
+  </si>
+  <si>
+    <t>R-BLD*</t>
   </si>
 </sst>
 </file>
@@ -1758,7 +1758,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1817,7 +1817,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>77</v>
@@ -1849,14 +1849,14 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Apt</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>"RSDSH_"&amp;L8</f>
         <v>RSDSH_Apt</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="2">
         <v>2019</v>
@@ -1898,14 +1898,14 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Att</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>"RSDSH_"&amp;L10</f>
         <v>RSDSH_Att</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="2">
         <v>2019</v>
@@ -1947,14 +1947,14 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Det</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>"RSDSH_"&amp;L12</f>
         <v>RSDSH_Det</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F12" s="2">
         <v>2019</v>
@@ -2009,7 +2009,7 @@
         <v>RSDWH_Apt</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" s="2">
         <v>2019</v>
@@ -2053,7 +2053,7 @@
         <v>RSDWH_Att</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16" s="2">
         <v>2019</v>
@@ -2097,7 +2097,7 @@
         <v>RSDWH_Det</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18" s="2">
         <v>2019</v>
@@ -2166,7 +2166,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>77</v>
@@ -2186,16 +2186,16 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="F24" s="2">
         <v>2019</v>

</xml_diff>

<commit_message>
Update HVO UP UC and add Cooker = Buildings
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_RSD_UnitBoilers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7087BA65-58F7-4A18-A06A-598B7B6CD0FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A52B6A0-7498-4EA5-8ABE-8419DF4B21B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -1758,7 +1758,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2150,7 +2150,9 @@
       <c r="L20" s="4"/>
     </row>
     <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="G22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">

</xml_diff>

<commit_message>
Recheck Coal constraint and Some Fireplaces restricted by buildings
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_RSD_UnitBoilers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA93316-2C40-4AE2-AFD5-99AC3F0CF371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439392BC-3533-44C3-B79A-014DF792A64F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -365,10 +365,10 @@
     <t>R*</t>
   </si>
   <si>
-    <t>*,-*RTFT*,-R*FPL*</t>
-  </si>
-  <si>
     <t>R-BLD*</t>
+  </si>
+  <si>
+    <t>*,-*RTFT*,-R*FPL_N1</t>
   </si>
 </sst>
 </file>
@@ -1749,7 +1749,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1840,7 +1840,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Apt</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>"RSDSH_"&amp;L8</f>
@@ -1889,7 +1889,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Att</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>"RSDSH_"&amp;L10</f>
@@ -1938,7 +1938,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Det</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>"RSDSH_"&amp;L12</f>
@@ -2208,7 +2208,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C25" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H25" s="2">
         <v>-1</v>

</xml_diff>